<commit_message>
fixes to combined method
</commit_message>
<xml_diff>
--- a/proj2-stats.xlsx
+++ b/proj2-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Documents\GitHub\ACS-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4BB30A-B822-43CC-B541-5A0D4C169846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D57DBB-DC03-4FB3-93A5-F74819D53F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{E3454171-55DD-475B-BE2E-6CDBA9D0AFB3}"/>
   </bookViews>
@@ -1286,34 +1286,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.70954E-2</c:v>
+                  <c:v>5.7773299999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.121548</c:v>
+                  <c:v>1.7118499999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.343061</c:v>
+                  <c:v>3.2907699999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98537200000000003</c:v>
+                  <c:v>7.5818800000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7542199999999999</c:v>
+                  <c:v>0.162605</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7063799999999998</c:v>
+                  <c:v>0.21192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.82422</c:v>
+                  <c:v>0.366394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4815899999999997</c:v>
+                  <c:v>0.70277599999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.3880299999999997</c:v>
+                  <c:v>0.72885</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.958399999999999</c:v>
+                  <c:v>0.88424800000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2292,34 +2292,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.1648699999999994E-3</c:v>
+                  <c:v>5.8496399999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1878699999999998E-3</c:v>
+                  <c:v>6.6879400000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0086299999999999E-2</c:v>
+                  <c:v>1.3018699999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6383700000000001E-2</c:v>
+                  <c:v>8.1160299999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7828200000000001E-2</c:v>
+                  <c:v>9.8357800000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1585599999999997E-2</c:v>
+                  <c:v>1.0606600000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.7238699999999993E-2</c:v>
+                  <c:v>1.0413199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.1920500000000002E-2</c:v>
+                  <c:v>1.4773E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12346699999999999</c:v>
+                  <c:v>2.6062200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17847299999999999</c:v>
+                  <c:v>2.15956E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9701,7 +9701,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Cache Miss'!$A$4</c:f>
+              <c:f>Combined!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9736,7 +9736,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Cache Miss'!$B$4:$B$13</c:f>
+              <c:f>Combined!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -9775,39 +9775,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Cache Miss'!$C$4:$C$13</c:f>
+              <c:f>Combined!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.52319E-2</c:v>
+                  <c:v>1.11633E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47889500000000002</c:v>
+                  <c:v>8.9401099999999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5933600000000001</c:v>
+                  <c:v>1.4279099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6827999999999999</c:v>
+                  <c:v>2.5055500000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1981299999999999</c:v>
+                  <c:v>3.9445800000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.556699999999999</c:v>
+                  <c:v>8.7393200000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.0395</c:v>
+                  <c:v>0.12521599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.9193</c:v>
+                  <c:v>0.16814100000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42.594799999999999</c:v>
+                  <c:v>0.22578500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>58.831299999999999</c:v>
+                  <c:v>0.30410900000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11054,34 +11054,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.153361</c:v>
+                  <c:v>5.0095099999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57850699999999999</c:v>
+                  <c:v>7.5114399999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3575900000000001</c:v>
+                  <c:v>0.204151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.31637</c:v>
+                  <c:v>0.26647500000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.7523300000000002</c:v>
+                  <c:v>0.74996700000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3150300000000001</c:v>
+                  <c:v>0.82633800000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.4945599999999999</c:v>
+                  <c:v>1.35978</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9648299999999992</c:v>
+                  <c:v>1.9461999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.92</c:v>
+                  <c:v>3.3914900000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.444099999999999</c:v>
+                  <c:v>4.3013399999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11177,34 +11177,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.70954E-2</c:v>
+                  <c:v>5.7773299999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.121548</c:v>
+                  <c:v>1.7118499999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.343061</c:v>
+                  <c:v>3.2907699999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98537200000000003</c:v>
+                  <c:v>7.5818800000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7542199999999999</c:v>
+                  <c:v>0.162605</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7063799999999998</c:v>
+                  <c:v>0.21192</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.82422</c:v>
+                  <c:v>0.366394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4815899999999997</c:v>
+                  <c:v>0.70277599999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.3880299999999997</c:v>
+                  <c:v>0.72885</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.958399999999999</c:v>
+                  <c:v>0.88424800000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11300,34 +11300,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>8.1648699999999994E-3</c:v>
+                  <c:v>5.8496399999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.1878699999999998E-3</c:v>
+                  <c:v>6.6879400000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0086299999999999E-2</c:v>
+                  <c:v>1.3018699999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6383700000000001E-2</c:v>
+                  <c:v>8.1160299999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7828200000000001E-2</c:v>
+                  <c:v>9.8357800000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1585599999999997E-2</c:v>
+                  <c:v>1.0606600000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.7238699999999993E-2</c:v>
+                  <c:v>1.0413199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.1920500000000002E-2</c:v>
+                  <c:v>1.4773E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12346699999999999</c:v>
+                  <c:v>2.6062200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.17847299999999999</c:v>
+                  <c:v>2.15956E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13098,34 +13098,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.29349E-3</c:v>
+                  <c:v>1.11633E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3555599999999997E-3</c:v>
+                  <c:v>8.9401099999999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8766799999999999E-2</c:v>
+                  <c:v>1.4279099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.3843500000000001E-2</c:v>
+                  <c:v>2.5055500000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18758</c:v>
+                  <c:v>3.9445800000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59848900000000005</c:v>
+                  <c:v>8.7393200000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3577999999999999</c:v>
+                  <c:v>0.12521599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5880800000000002</c:v>
+                  <c:v>0.16814100000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4394400000000003</c:v>
+                  <c:v>0.22578500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9380600000000001</c:v>
+                  <c:v>0.30410900000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13990,34 +13990,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.29349E-3</c:v>
+                  <c:v>1.11633E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3555599999999997E-3</c:v>
+                  <c:v>8.9401099999999994E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8766799999999999E-2</c:v>
+                  <c:v>1.4279099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.3843500000000001E-2</c:v>
+                  <c:v>2.5055500000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18758</c:v>
+                  <c:v>3.9445800000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59848900000000005</c:v>
+                  <c:v>8.7393200000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3577999999999999</c:v>
+                  <c:v>0.12521599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5880800000000002</c:v>
+                  <c:v>0.16814100000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4394400000000003</c:v>
+                  <c:v>0.22578500000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9380600000000001</c:v>
+                  <c:v>0.30410900000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17787,34 +17787,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.153361</c:v>
+                  <c:v>5.0095099999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57850699999999999</c:v>
+                  <c:v>7.5114399999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3575900000000001</c:v>
+                  <c:v>0.204151</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.31637</c:v>
+                  <c:v>0.26647500000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.7523300000000002</c:v>
+                  <c:v>0.74996700000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.3150300000000001</c:v>
+                  <c:v>0.82633800000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.4945599999999999</c:v>
+                  <c:v>1.35978</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9648299999999992</c:v>
+                  <c:v>1.9461999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.92</c:v>
+                  <c:v>3.3914900000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.444099999999999</c:v>
+                  <c:v>4.3013399999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31298,16 +31298,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -31739,13 +31739,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -32170,7 +32170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D2A3649-CE09-4626-BDCC-929B809EAA68}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
@@ -34371,7 +34371,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34413,7 +34413,7 @@
         <v>200</v>
       </c>
       <c r="C4">
-        <v>2.29349E-3</v>
+        <v>1.11633E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -34424,7 +34424,7 @@
         <v>400</v>
       </c>
       <c r="C5">
-        <v>6.3555599999999997E-3</v>
+        <v>8.9401099999999994E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -34435,7 +34435,7 @@
         <v>600</v>
       </c>
       <c r="C6">
-        <v>2.8766799999999999E-2</v>
+        <v>1.4279099999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -34446,7 +34446,7 @@
         <v>800</v>
       </c>
       <c r="C7">
-        <v>8.3843500000000001E-2</v>
+        <v>2.5055500000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -34457,7 +34457,7 @@
         <v>1000</v>
       </c>
       <c r="C8">
-        <v>0.18758</v>
+        <v>3.9445800000000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -34468,7 +34468,7 @@
         <v>1200</v>
       </c>
       <c r="C9">
-        <v>0.59848900000000005</v>
+        <v>8.7393200000000004E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -34479,7 +34479,7 @@
         <v>1400</v>
       </c>
       <c r="C10">
-        <v>1.3577999999999999</v>
+        <v>0.12521599999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -34490,7 +34490,7 @@
         <v>1600</v>
       </c>
       <c r="C11">
-        <v>2.5880800000000002</v>
+        <v>0.16814100000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -34501,7 +34501,7 @@
         <v>1800</v>
       </c>
       <c r="C12">
-        <v>4.4394400000000003</v>
+        <v>0.22578500000000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -34512,7 +34512,7 @@
         <v>2000</v>
       </c>
       <c r="C13">
-        <v>6.9380600000000001</v>
+        <v>0.30410900000000002</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -34625,13 +34625,13 @@
         <v>1000</v>
       </c>
       <c r="C22">
-        <v>0.153361</v>
+        <v>5.0095099999999997E-2</v>
       </c>
       <c r="D22">
-        <v>1.70954E-2</v>
+        <v>5.7773299999999998E-3</v>
       </c>
       <c r="E22">
-        <v>8.1648699999999994E-3</v>
+        <v>5.8496399999999997E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -34642,13 +34642,13 @@
         <v>2000</v>
       </c>
       <c r="C23">
-        <v>0.57850699999999999</v>
+        <v>7.5114399999999998E-2</v>
       </c>
       <c r="D23">
-        <v>0.121548</v>
+        <v>1.7118499999999998E-2</v>
       </c>
       <c r="E23">
-        <v>6.1878699999999998E-3</v>
+        <v>6.6879400000000001E-4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -34659,13 +34659,13 @@
         <v>3000</v>
       </c>
       <c r="C24">
-        <v>1.3575900000000001</v>
+        <v>0.204151</v>
       </c>
       <c r="D24">
-        <v>0.343061</v>
+        <v>3.2907699999999998E-2</v>
       </c>
       <c r="E24">
-        <v>1.0086299999999999E-2</v>
+        <v>1.3018699999999999E-3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -34676,13 +34676,13 @@
         <v>4000</v>
       </c>
       <c r="C25">
-        <v>2.31637</v>
+        <v>0.26647500000000002</v>
       </c>
       <c r="D25">
-        <v>0.98537200000000003</v>
+        <v>7.5818800000000006E-2</v>
       </c>
       <c r="E25">
-        <v>1.6383700000000001E-2</v>
+        <v>8.1160299999999998E-3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -34693,13 +34693,13 @@
         <v>5000</v>
       </c>
       <c r="C26">
-        <v>3.7523300000000002</v>
+        <v>0.74996700000000005</v>
       </c>
       <c r="D26">
-        <v>1.7542199999999999</v>
+        <v>0.162605</v>
       </c>
       <c r="E26">
-        <v>2.7828200000000001E-2</v>
+        <v>9.8357800000000006E-3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -34710,13 +34710,13 @@
         <v>6000</v>
       </c>
       <c r="C27">
-        <v>5.3150300000000001</v>
+        <v>0.82633800000000002</v>
       </c>
       <c r="D27">
-        <v>2.7063799999999998</v>
+        <v>0.21192</v>
       </c>
       <c r="E27">
-        <v>6.1585599999999997E-2</v>
+        <v>1.0606600000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -34727,13 +34727,13 @@
         <v>7000</v>
       </c>
       <c r="C28">
-        <v>9.4945599999999999</v>
+        <v>1.35978</v>
       </c>
       <c r="D28">
-        <v>3.82422</v>
+        <v>0.366394</v>
       </c>
       <c r="E28">
-        <v>7.7238699999999993E-2</v>
+        <v>1.0413199999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -34744,13 +34744,13 @@
         <v>8000</v>
       </c>
       <c r="C29">
-        <v>8.9648299999999992</v>
+        <v>1.9461999999999999</v>
       </c>
       <c r="D29">
-        <v>5.4815899999999997</v>
+        <v>0.70277599999999996</v>
       </c>
       <c r="E29">
-        <v>9.1920500000000002E-2</v>
+        <v>1.4773E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -34761,13 +34761,13 @@
         <v>9000</v>
       </c>
       <c r="C30">
-        <v>15.92</v>
+        <v>3.3914900000000001</v>
       </c>
       <c r="D30">
-        <v>7.3880299999999997</v>
+        <v>0.72885</v>
       </c>
       <c r="E30">
-        <v>0.12346699999999999</v>
+        <v>2.6062200000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -34778,13 +34778,13 @@
         <v>10000</v>
       </c>
       <c r="C31">
-        <v>21.444099999999999</v>
+        <v>4.3013399999999997</v>
       </c>
       <c r="D31">
-        <v>10.958399999999999</v>
+        <v>0.88424800000000003</v>
       </c>
       <c r="E31">
-        <v>0.17847299999999999</v>
+        <v>2.15956E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>